<commit_message>
ExtentReports added.log created. helper class methods created for scrrenshot and date time
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -17,10 +17,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>chinmaya</t>
+    <t>inspiron1545</t>
   </si>
   <si>
-    <t>inspiron1545</t>
+    <t>chinmaya</t>
   </si>
 </sst>
 </file>
@@ -364,9 +364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -376,10 +374,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>